<commit_message>
Created housing matters mobile site analysis
I did half of the website - James did the other half
Callum took the desktop page
</commit_message>
<xml_diff>
--- a/Housing Matters/Housing Matters.xlsx
+++ b/Housing Matters/Housing Matters.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27021"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{616A3638-6486-4667-A74A-8D89BA31B2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DB9D62B-161B-48A6-805E-E9189E6B94EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Luke" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Studio Blog</t>
   </si>
@@ -53,52 +53,106 @@
     <t>Week Number</t>
   </si>
   <si>
+    <t>This weeks task?</t>
+  </si>
+  <si>
+    <t>What was achieved?</t>
+  </si>
+  <si>
+    <t>What is to be done next week/carried over?</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>09/10 - 16/10</t>
+  </si>
+  <si>
+    <t>Email Alice to schedule a meeting and get access to assets</t>
+  </si>
+  <si>
+    <t>Email was sent with meeting being scheduled</t>
+  </si>
+  <si>
+    <t>Meeting for introduction and discuss matters moving forward</t>
+  </si>
+  <si>
+    <t>Assets did not arrive</t>
+  </si>
+  <si>
+    <t>16/10 - 23/10</t>
+  </si>
+  <si>
+    <t>Meeting with Alice and look through assets</t>
+  </si>
+  <si>
+    <t>Meeting with Kat and Andrew and assets arrived for us to look through - also got access to google analytics</t>
+  </si>
+  <si>
+    <t>Create user personas and journey for someone seeking to to donate and a client, also look through assets provided to us</t>
+  </si>
+  <si>
+    <t>Mentioned Jasmine rebranded the website and we may have a meeting with her soon</t>
+  </si>
+  <si>
+    <t>23/10 - 30/10</t>
+  </si>
+  <si>
+    <t>Created a User Persona and Journey for someone donating and another seeking advice, looked through assets as well as google analytics</t>
+  </si>
+  <si>
+    <t>Meeting as group to discuss our personas and user journey before meeting on Tuesday</t>
+  </si>
+  <si>
+    <t>Meeting with Jasmine has been confirmed, Alice will also be joining</t>
+  </si>
+  <si>
+    <t>30/10 - 06/11</t>
+  </si>
+  <si>
+    <t>Create user journey and persona for a potential partner. analyse half of mobile site</t>
+  </si>
+  <si>
+    <t>Created user persona and journey, meeting with Jasmine, Alice and Kat, Created project plan, created website analysis for my portion</t>
+  </si>
+  <si>
+    <t>Weekly meeting, competitor analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile pages to analyse are About Us (our partnerships - new us), Helpful resources, home page, donate </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>What was the Task?</t>
   </si>
   <si>
-    <t>What was achieved?</t>
-  </si>
-  <si>
     <t>What is to be done next week?</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Email Alice to schedule a meeting and get access to assets</t>
-  </si>
-  <si>
-    <t>Email was sent with meeting being scheduled - assets did not arrive</t>
-  </si>
-  <si>
-    <t>Meeting for introduction and discuss matters moving forward</t>
-  </si>
-  <si>
-    <t>Meeting with Alice and look through assets</t>
-  </si>
-  <si>
-    <t>Meeting with Kat and Andrew and assets arrived for us to look through - also got access to google analytics</t>
-  </si>
-  <si>
-    <t>Create user personas and journey for someone seeking to to donate and a client, also look through assets provided to us</t>
-  </si>
-  <si>
-    <t>Mentioned Jasmine rebranded the website and we may have a meeting with her soon</t>
-  </si>
-  <si>
-    <t>Created a User Persona and Journey for someone donating and another seeking advice, looked through assets as well as google analytics</t>
-  </si>
-  <si>
-    <t>Meeting as group to discuss our personas and user journey before meeting on Tuesday</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Schedule Weekly Meetings</t>
   </si>
   <si>
-    <t>Create User Personas (client &amp; Fundraiser)</t>
+    <t>Assets arrived later on in the weak</t>
+  </si>
+  <si>
+    <t>Create user personas and journey for a HPI looking to to donate and a client, also look through assets provided to us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 user journey maps and 2 user personas on client and donater </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting as group to discuss our personas and user journey before meeting on Tuesday. Also create a </t>
+  </si>
+  <si>
+    <t>Create a fundraiser person and user journey map. Analyse half of the mobile site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About us (Top 4), contact us, your stories, our impact. </t>
+  </si>
+  <si>
+    <t>Funder - Mission statements, vissions values, how they can contact, case studies.</t>
   </si>
 </sst>
 </file>
@@ -718,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F4910B0-AB8A-4E8B-9A1F-44B156E3F234}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -813,19 +867,21 @@
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" ht="60" customHeight="1">
-      <c r="B6" s="7">
-        <v>1</v>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -834,20 +890,20 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="60" customHeight="1">
-      <c r="B7" s="7">
-        <v>2</v>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -857,19 +913,21 @@
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="60" customHeight="1">
-      <c r="B8" s="7">
-        <v>3</v>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -878,13 +936,21 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" ht="60" customHeight="1">
-      <c r="B9" s="7">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -930,7 +996,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1116,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1226,7 +1292,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1338,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C013432C-2912-4894-B87E-8032BCE8F6B3}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1347,7 +1413,7 @@
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
@@ -1412,11 +1478,17 @@
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1429,11 +1501,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1446,11 +1524,17 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1462,10 +1546,18 @@
       <c r="B8" s="7">
         <v>3</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -1479,9 +1571,15 @@
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -1492,7 +1590,9 @@
       <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1526,7 +1626,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
       <c r="F12" s="9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>

</xml_diff>